<commit_message>
updates to clear issues
</commit_message>
<xml_diff>
--- a/be-allergyintolerance.xlsx
+++ b/be-allergyintolerance.xlsx
@@ -156,8 +156,8 @@
     <t>Substances include, but are not limited to: a therapeutic substance administered correctly at an appropriate dosage for the individual; food; material derived from plants or animals; or venom from insect stings.</t>
   </si>
   <si>
-    <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.div.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}ait-1:AllergyIntolerance.clinicalStatus SHALL be present if verificationStatus is not entered-in-error. {verificationStatus='entered-in-error' or clinicalStatus.exists()}ait-2:AllergyIntolerance.clinicalStatus SHALL NOT be present if verification Status is entered-in-error {verificationStatus!='entered-in-error' or clinicalStatus.empty()}</t>
+    <t>ait-1:AllergyIntolerance.clinicalStatus SHALL be present if verificationStatus is not entered-in-error. {verificationStatus.coding.where(system = 'http://terminology.hl7.org/CodeSystem/allergyintolerance-verification' and code = 'entered-in-error').exists() or clinicalStatus.exists()}
+ait-2:AllergyIntolerance.clinicalStatus SHALL NOT be present if verification Status is entered-in-error {verificationStatus.coding.where(system = 'http://terminology.hl7.org/CodeSystem/allergyintolerance-verification' and code = 'entered-in-error').empty() or clinicalStatus.empty()}dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
   </si>
   <si>
     <t>Observation[classCode=OBS, moodCode=EVN]</t>
@@ -172,7 +172,7 @@
     <t>Y</t>
   </si>
   <si>
-    <t xml:space="preserve">id
+    <t xml:space="preserve">string
 </t>
   </si>
   <si>
@@ -204,6 +204,10 @@
     <t>Resource.meta</t>
   </si>
   <si>
+    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+</t>
+  </si>
+  <si>
     <t>AllergyIntolerance.implicitRules</t>
   </si>
   <si>
@@ -326,6 +330,10 @@
     <t>DomainResource.extension</t>
   </si>
   <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
     <t>AllergyIntolerance.modifierExtension</t>
   </si>
   <si>
@@ -390,7 +398,7 @@
     <t>required</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/allergyintolerance-clinical|4.0.0</t>
+    <t>http://hl7.org/fhir/ValueSet/allergyintolerance-clinical|4.0.1</t>
   </si>
   <si>
     <t>ait-1
@@ -418,7 +426,7 @@
     <t>Assertion about certainty associated with a propensity, or potential risk, of a reaction to the identified substance.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/allergyintolerance-verification|4.0.0</t>
+    <t>http://hl7.org/fhir/ValueSet/allergyintolerance-verification|4.0.1</t>
   </si>
   <si>
     <t>Observation ACT .inboundRelationship[typeCode=COMP].source[classCode=OBS, code="verificationStatus", moodCode=EVN].value</t>
@@ -443,7 +451,7 @@
     <t>Identification of the underlying physiological mechanism for a Reaction Risk.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/allergy-intolerance-type|4.0.0</t>
+    <t>http://hl7.org/fhir/ValueSet/allergy-intolerance-type|4.0.1</t>
   </si>
   <si>
     <t>code</t>
@@ -474,7 +482,7 @@
     <t>Category of an identified substance associated with allergies or intolerances.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/allergy-intolerance-category|4.0.0</t>
+    <t>http://hl7.org/fhir/ValueSet/allergy-intolerance-category|4.0.1</t>
   </si>
   <si>
     <t>value &lt; IntoleranceValue (Agent)</t>
@@ -502,7 +510,7 @@
     <t>Estimate of the potential clinical harm, or seriousness, of a reaction to an identified substance.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/allergy-intolerance-criticality|4.0.0</t>
+    <t>http://hl7.org/fhir/ValueSet/allergy-intolerance-criticality|4.0.1</t>
   </si>
   <si>
     <t>inboundRelationship[typeCode=SUBJ].source[classCode=OBS, moodCode=EVN, code=SEV, value &lt;= SeverityObservation (Severity Level)]</t>
@@ -743,18 +751,10 @@
     <t>Details about each adverse reaction event linked to exposure to the identified substance.</t>
   </si>
   <si>
-    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-</t>
-  </si>
-  <si>
     <t>outBoundRelationship[typeCode=SUBJ].target[classCode=OBS, moodCode=EVN, code &lt;= CommonClinicalObservationType, value &lt;= ObservationValue (Reaction Type)]</t>
   </si>
   <si>
     <t>AllergyIntolerance.reaction.id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string
-</t>
   </si>
   <si>
     <t>Unique id for inter-element referencing</t>
@@ -887,7 +887,7 @@
     <t>Clinical assessment of the severity of a reaction event as a whole, potentially considering multiple different manifestations.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/reaction-event-severity|4.0.0</t>
+    <t>http://hl7.org/fhir/ValueSet/reaction-event-severity|4.0.1</t>
   </si>
   <si>
     <t>AllergyIntolerance.reaction.exposureRoute</t>
@@ -1544,7 +1544,7 @@
         <v>42</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>42</v>
@@ -1558,7 +1558,7 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -1581,16 +1581,16 @@
         <v>50</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
@@ -1640,7 +1640,7 @@
         <v>42</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AF5" t="s" s="2">
         <v>40</v>
@@ -1652,7 +1652,7 @@
         <v>42</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ5" t="s" s="2">
         <v>42</v>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -1689,16 +1689,16 @@
         <v>42</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" t="s" s="2">
@@ -1724,13 +1724,13 @@
         <v>42</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Z6" t="s" s="2">
         <v>42</v>
@@ -1748,7 +1748,7 @@
         <v>42</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>40</v>
@@ -1760,7 +1760,7 @@
         <v>42</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ6" t="s" s="2">
         <v>42</v>
@@ -1774,11 +1774,11 @@
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s" s="2">
@@ -1797,16 +1797,16 @@
         <v>42</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" t="s" s="2">
@@ -1856,7 +1856,7 @@
         <v>42</v>
       </c>
       <c r="AE7" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AF7" t="s" s="2">
         <v>40</v>
@@ -1868,10 +1868,10 @@
         <v>42</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ7" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AK7" t="s" s="2">
         <v>42</v>
@@ -1882,11 +1882,11 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" t="s" s="2">
@@ -1905,16 +1905,16 @@
         <v>42</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -1964,7 +1964,7 @@
         <v>42</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>40</v>
@@ -1979,7 +1979,7 @@
         <v>42</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK8" t="s" s="2">
         <v>42</v>
@@ -1990,11 +1990,11 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
@@ -2013,16 +2013,16 @@
         <v>42</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
@@ -2072,7 +2072,7 @@
         <v>42</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>40</v>
@@ -2084,10 +2084,10 @@
         <v>42</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK9" t="s" s="2">
         <v>42</v>
@@ -2098,11 +2098,11 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
@@ -2121,19 +2121,19 @@
         <v>42</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N10" t="s" s="2">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="O10" t="s" s="2">
         <v>42</v>
@@ -2182,7 +2182,7 @@
         <v>42</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>40</v>
@@ -2194,10 +2194,10 @@
         <v>42</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK10" t="s" s="2">
         <v>42</v>
@@ -2208,7 +2208,7 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -2231,19 +2231,19 @@
         <v>50</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="N11" t="s" s="2">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="O11" t="s" s="2">
         <v>42</v>
@@ -2292,7 +2292,7 @@
         <v>42</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>40</v>
@@ -2304,21 +2304,21 @@
         <v>42</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -2341,16 +2341,16 @@
         <v>50</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
@@ -2376,13 +2376,13 @@
         <v>42</v>
       </c>
       <c r="W12" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="X12" t="s" s="2">
         <v>118</v>
       </c>
-      <c r="X12" t="s" s="2">
-        <v>116</v>
-      </c>
       <c r="Y12" t="s" s="2">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="Z12" t="s" s="2">
         <v>42</v>
@@ -2400,7 +2400,7 @@
         <v>42</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>40</v>
@@ -2409,16 +2409,16 @@
         <v>49</v>
       </c>
       <c r="AH12" t="s" s="2">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="AL12" t="s" s="2">
         <v>42</v>
@@ -2426,7 +2426,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2449,16 +2449,16 @@
         <v>50</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
@@ -2484,13 +2484,13 @@
         <v>42</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Y13" t="s" s="2">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>42</v>
@@ -2508,7 +2508,7 @@
         <v>42</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>40</v>
@@ -2517,16 +2517,16 @@
         <v>49</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="AL13" t="s" s="2">
         <v>42</v>
@@ -2534,11 +2534,11 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
@@ -2557,16 +2557,16 @@
         <v>50</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -2592,13 +2592,13 @@
         <v>42</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>42</v>
@@ -2616,7 +2616,7 @@
         <v>42</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>40</v>
@@ -2628,25 +2628,25 @@
         <v>42</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
@@ -2665,16 +2665,16 @@
         <v>50</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
@@ -2700,13 +2700,13 @@
         <v>42</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>42</v>
@@ -2724,7 +2724,7 @@
         <v>42</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>40</v>
@@ -2736,25 +2736,25 @@
         <v>42</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
@@ -2773,16 +2773,16 @@
         <v>50</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -2808,13 +2808,13 @@
         <v>42</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>42</v>
@@ -2832,7 +2832,7 @@
         <v>42</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>40</v>
@@ -2844,25 +2844,25 @@
         <v>42</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
@@ -2881,16 +2881,16 @@
         <v>50</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" t="s" s="2">
@@ -2916,13 +2916,13 @@
         <v>42</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>42</v>
@@ -2940,7 +2940,7 @@
         <v>42</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>40</v>
@@ -2952,25 +2952,25 @@
         <v>42</v>
       </c>
       <c r="AI17" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
@@ -2989,13 +2989,13 @@
         <v>50</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -3046,7 +3046,7 @@
         <v>42</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>49</v>
@@ -3058,21 +3058,21 @@
         <v>42</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3095,13 +3095,13 @@
         <v>42</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -3152,7 +3152,7 @@
         <v>42</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>40</v>
@@ -3164,13 +3164,13 @@
         <v>42</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>42</v>
@@ -3178,7 +3178,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3201,13 +3201,13 @@
         <v>42</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -3258,7 +3258,7 @@
         <v>42</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>40</v>
@@ -3270,13 +3270,13 @@
         <v>42</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>42</v>
@@ -3284,7 +3284,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3307,13 +3307,13 @@
         <v>42</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -3364,7 +3364,7 @@
         <v>42</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>40</v>
@@ -3376,25 +3376,25 @@
         <v>42</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
@@ -3413,13 +3413,13 @@
         <v>42</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -3470,7 +3470,7 @@
         <v>42</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>40</v>
@@ -3482,13 +3482,13 @@
         <v>42</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>42</v>
@@ -3496,11 +3496,11 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
@@ -3519,16 +3519,16 @@
         <v>50</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
@@ -3578,7 +3578,7 @@
         <v>42</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>40</v>
@@ -3590,21 +3590,21 @@
         <v>42</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3627,16 +3627,16 @@
         <v>42</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
@@ -3686,7 +3686,7 @@
         <v>42</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>40</v>
@@ -3698,10 +3698,10 @@
         <v>42</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>42</v>
@@ -3712,7 +3712,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3735,16 +3735,16 @@
         <v>42</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
@@ -3794,7 +3794,7 @@
         <v>42</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>40</v>
@@ -3806,10 +3806,10 @@
         <v>42</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>42</v>
@@ -3820,7 +3820,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3843,13 +3843,13 @@
         <v>42</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -3900,7 +3900,7 @@
         <v>42</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>40</v>
@@ -3912,10 +3912,10 @@
         <v>42</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>227</v>
+        <v>61</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AK26" t="s" s="2">
         <v>42</v>
@@ -3926,7 +3926,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -3949,7 +3949,7 @@
         <v>42</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>230</v>
+        <v>51</v>
       </c>
       <c r="K27" t="s" s="2">
         <v>231</v>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
@@ -4055,16 +4055,16 @@
         <v>42</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L28" t="s" s="2">
         <v>236</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4126,7 +4126,7 @@
         <v>42</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="AJ28" t="s" s="2">
         <v>234</v>
@@ -4163,7 +4163,7 @@
         <v>50</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K29" t="s" s="2">
         <v>240</v>
@@ -4172,10 +4172,10 @@
         <v>241</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="O29" t="s" s="2">
         <v>42</v>
@@ -4236,10 +4236,10 @@
         <v>42</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>42</v>
@@ -4273,7 +4273,7 @@
         <v>42</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="K30" t="s" s="2">
         <v>244</v>
@@ -4344,7 +4344,7 @@
         <v>42</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>250</v>
@@ -4381,7 +4381,7 @@
         <v>42</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="K31" t="s" s="2">
         <v>253</v>
@@ -4416,7 +4416,7 @@
         <v>42</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="X31" s="2"/>
       <c r="Y31" t="s" s="2">
@@ -4450,10 +4450,10 @@
         <v>42</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>42</v>
@@ -4487,7 +4487,7 @@
         <v>42</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>230</v>
+        <v>51</v>
       </c>
       <c r="K32" t="s" s="2">
         <v>260</v>
@@ -4558,7 +4558,7 @@
         <v>42</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>263</v>
@@ -4595,7 +4595,7 @@
         <v>42</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="K33" t="s" s="2">
         <v>265</v>
@@ -4664,10 +4664,10 @@
         <v>42</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>42</v>
@@ -4701,7 +4701,7 @@
         <v>42</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K34" t="s" s="2">
         <v>269</v>
@@ -4736,7 +4736,7 @@
         <v>42</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="X34" t="s" s="2">
         <v>272</v>
@@ -4772,10 +4772,10 @@
         <v>42</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>42</v>
@@ -4809,7 +4809,7 @@
         <v>42</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="K35" t="s" s="2">
         <v>275</v>
@@ -4880,7 +4880,7 @@
         <v>42</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>280</v>
@@ -4917,7 +4917,7 @@
         <v>42</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="K36" t="s" s="2">
         <v>282</v>
@@ -4988,10 +4988,10 @@
         <v>42</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>42</v>

</xml_diff>